<commit_message>
updated the map locations and latest KML files
</commit_message>
<xml_diff>
--- a/Data/Covid2019/SA_data_archive/Gauteng/sub-district map locations.xlsx
+++ b/Data/Covid2019/SA_data_archive/Gauteng/sub-district map locations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="109">
   <si>
     <t>Diepsloot</t>
   </si>
@@ -263,6 +263,84 @@
   </si>
   <si>
     <t>Weilers Farm</t>
+  </si>
+  <si>
+    <t>Ga-Rankuwa</t>
+  </si>
+  <si>
+    <t>-25.6041667,28.0052778</t>
+  </si>
+  <si>
+    <t>Tshwane 1</t>
+  </si>
+  <si>
+    <t>Mapopane</t>
+  </si>
+  <si>
+    <t>Winderveldt</t>
+  </si>
+  <si>
+    <t>Soshanguve</t>
+  </si>
+  <si>
+    <t>Rosslyn</t>
+  </si>
+  <si>
+    <t>Karenpark</t>
+  </si>
+  <si>
+    <t>Wonderboom</t>
+  </si>
+  <si>
+    <t>Akasia</t>
+  </si>
+  <si>
+    <t>Nina Park</t>
+  </si>
+  <si>
+    <t>Orchards</t>
+  </si>
+  <si>
+    <t>Amandasig</t>
+  </si>
+  <si>
+    <t>Theresa Park</t>
+  </si>
+  <si>
+    <t>Pretoria North</t>
+  </si>
+  <si>
+    <t>Hammanskraal</t>
+  </si>
+  <si>
+    <t>Temba</t>
+  </si>
+  <si>
+    <t>Suurman</t>
+  </si>
+  <si>
+    <t>Dilopye</t>
+  </si>
+  <si>
+    <t>Stinkwater</t>
+  </si>
+  <si>
+    <t>Ramotse</t>
+  </si>
+  <si>
+    <t>New Eesterus</t>
+  </si>
+  <si>
+    <t>Kameeldrit</t>
+  </si>
+  <si>
+    <t>Pyramid/Rooiwal</t>
+  </si>
+  <si>
+    <t>Do</t>
+  </si>
+  <si>
+    <t>Tshwane 2</t>
   </si>
 </sst>
 </file>
@@ -304,10 +382,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1040,6 +1119,166 @@
         <v>50</v>
       </c>
     </row>
+    <row r="39" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>